<commit_message>
Updated Congigs based on review comments on Sprint6 from client
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\PROJECTS\MOSIP\Desk Items\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4FEEF03-7D6E-40CF-BEF9-9CFB628D620D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5450F228-A8D5-4D3B-A87E-B84478F6941B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -800,15 +800,6 @@
     <t>Setup PDF template for Full e-KYC</t>
   </si>
   <si>
-    <t>Setup time zone for a country/state</t>
-  </si>
-  <si>
-    <t>UTC</t>
-  </si>
-  <si>
-    <t>UTC+1, UTC+5.30</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -964,6 +955,15 @@
   </si>
   <si>
     <t>1MB</t>
+  </si>
+  <si>
+    <t>Setup Priority between Fingerprint Image and Minutae when both are present in the input</t>
+  </si>
+  <si>
+    <t>Priority 1 and 2 for Fingerprint Image and Minutiae respectively</t>
+  </si>
+  <si>
+    <t>Priority 2 and 1 for Fingerprint Image and Minutiae respectively</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -2375,7 +2375,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>9</v>
@@ -2460,9 +2460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2537,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -2646,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="21" t="s">
@@ -2807,7 +2807,7 @@
       </c>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="58" t="s">
@@ -2960,7 +2960,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C27" s="60" t="s">
         <v>9</v>
@@ -2969,7 +2969,7 @@
         <v>43101</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F27" s="58" t="s">
         <v>12</v>
@@ -2981,13 +2981,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="21" t="s">
@@ -3085,7 +3085,7 @@
         <v>70</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G3" s="7"/>
     </row>
@@ -3123,7 +3123,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="55" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -3161,7 +3161,7 @@
         <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G14" s="7"/>
     </row>
@@ -3572,7 +3572,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>9</v>
@@ -3730,7 +3730,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>9</v>
@@ -3806,7 +3806,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C42" s="60" t="s">
         <v>9</v>
@@ -3815,7 +3815,7 @@
         <v>43101</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>12</v>
@@ -4845,13 +4845,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="21" t="s">
@@ -5914,7 +5914,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="64" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -6474,11 +6474,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" sqref="A1:G1"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6527,7 +6527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -6987,21 +6987,21 @@
       <c r="F26" s="11"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>206</v>
+      <c r="B27" s="46" t="s">
+        <v>232</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>208</v>
+      <c r="D27" s="49" t="s">
+        <v>233</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>234</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
@@ -7036,7 +7036,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="64" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -7073,13 +7073,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -7088,7 +7088,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="12"/>
@@ -7103,7 +7103,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="12"/>
@@ -7118,7 +7118,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="12"/>
@@ -7133,7 +7133,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="12"/>
@@ -7148,7 +7148,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="12"/>
@@ -7163,7 +7163,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="12"/>
@@ -7178,7 +7178,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C10" s="52"/>
       <c r="D10" s="12"/>

</xml_diff>

<commit_message>
Updated the Configuration List for Reg Processor
Updated the Configuration List for Reg Processor
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5450F228-A8D5-4D3B-A87E-B84478F6941B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF31D5FE-2487-4ACF-8325-A3D1499F5161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="245">
   <si>
     <r>
       <rPr>
@@ -530,11 +530,6 @@
     <t>Type of Notification to be triggered  &lt;Applicable for all modules&gt;</t>
   </si>
   <si>
-    <t>Email
-SMS
-Both</t>
-  </si>
-  <si>
     <t>Parent/Guardian Authentication Type</t>
   </si>
   <si>
@@ -546,9 +541,6 @@
   </si>
   <si>
     <t>The Age of Minor</t>
-  </si>
-  <si>
-    <t>5years</t>
   </si>
   <si>
     <t>1 - 10</t>
@@ -965,12 +957,51 @@
   <si>
     <t>Priority 2 and 1 for Fingerprint Image and Minutiae respectively</t>
   </si>
+  <si>
+    <t>EMAIL|SMS</t>
+  </si>
+  <si>
+    <t>EMAIL
+SMS
+EMAIL|SMS</t>
+  </si>
+  <si>
+    <t>Not Needed as we are removing the Functionality. There is no Wait for X hrs in MOSIP.</t>
+  </si>
+  <si>
+    <t>OK - Updated the Values</t>
+  </si>
+  <si>
+    <t>Not Needed because of Exact Match</t>
+  </si>
+  <si>
+    <t>OK - Change to Bio Dedupe Threshold</t>
+  </si>
+  <si>
+    <t>Not Needed Only One Limit is Requiered</t>
+  </si>
+  <si>
+    <t>Not Needed - Should be deleted if Virus Found</t>
+  </si>
+  <si>
+    <t>OK - Part of Master Data</t>
+  </si>
+  <si>
+    <t>Not Needed - Batch Job is removed</t>
+  </si>
+  <si>
+    <t>Not Needed - Landing Zone is removed</t>
+  </si>
+  <si>
+    <t>OK - Code Change Needed | Please Discuss with Shravan
+Not a Configurable Item in Admin will be a one time activity for a country</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1062,6 +1093,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1261,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1454,6 +1493,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1983,19 +2025,19 @@
       <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="35.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2049,7 @@
       <c r="G1" s="62"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2031,7 +2073,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2067,7 +2109,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2105,7 +2147,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2143,7 +2185,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2181,7 +2223,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2219,7 +2261,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2257,7 +2299,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2295,7 +2337,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -2313,7 +2355,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -2331,7 +2373,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -2351,7 +2393,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -2370,12 +2412,12 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>9</v>
@@ -2389,7 +2431,7 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -2408,7 +2450,7 @@
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -2425,7 +2467,7 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -2465,19 +2507,19 @@
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="16" customWidth="1"/>
     <col min="2" max="2" width="72" style="17" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="17" customWidth="1"/>
     <col min="5" max="5" width="16" style="17" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" style="18" customWidth="1"/>
     <col min="7" max="7" width="39" style="18" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>29</v>
       </c>
@@ -2488,7 +2530,7 @@
       <c r="F1" s="63"/>
       <c r="G1" s="63"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -2511,7 +2553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -2532,12 +2574,12 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="22" customFormat="1" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="20">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -2551,7 +2593,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -2572,7 +2614,7 @@
       </c>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -2593,7 +2635,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -2614,7 +2656,7 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -2635,7 +2677,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" s="22" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="22" customFormat="1" ht="104" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -2646,7 +2688,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="21" t="s">
@@ -2654,7 +2696,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -2671,7 +2713,7 @@
       </c>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -2688,7 +2730,7 @@
       </c>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -2705,7 +2747,7 @@
       </c>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -2722,7 +2764,7 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -2739,7 +2781,7 @@
       </c>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -2756,7 +2798,7 @@
       </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -2773,7 +2815,7 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -2790,7 +2832,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -2807,7 +2849,7 @@
       </c>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -2828,7 +2870,7 @@
       </c>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -2845,7 +2887,7 @@
       </c>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -2862,7 +2904,7 @@
       </c>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -2881,7 +2923,7 @@
       </c>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -2900,7 +2942,7 @@
       </c>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -2917,7 +2959,7 @@
       </c>
       <c r="G24" s="21"/>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -2936,7 +2978,7 @@
       </c>
       <c r="G25" s="21"/>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A26" s="57">
         <v>24</v>
       </c>
@@ -2947,7 +2989,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="58" t="s">
@@ -2955,12 +2997,12 @@
       </c>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>25</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C27" s="60" t="s">
         <v>9</v>
@@ -2969,25 +3011,25 @@
         <v>43101</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F27" s="58" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="56"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="20">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="21" t="s">
@@ -2995,7 +3037,7 @@
       </c>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="s">
         <v>66</v>
       </c>
@@ -3022,19 +3064,19 @@
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="60.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" style="17" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="60.54296875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="44.54296875" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
         <v>67</v>
       </c>
@@ -3045,7 +3087,7 @@
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
@@ -3068,7 +3110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3085,11 +3127,11 @@
         <v>70</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -3110,7 +3152,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="117" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -3123,11 +3165,11 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="55" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="65" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -3144,7 +3186,7 @@
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -3161,11 +3203,11 @@
         <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -3186,7 +3228,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3207,7 +3249,7 @@
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3228,7 +3270,7 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3249,7 +3291,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3270,7 +3312,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3291,7 +3333,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3306,11 +3348,11 @@
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -3329,7 +3371,7 @@
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -3346,7 +3388,7 @@
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -3363,7 +3405,7 @@
       </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -3380,7 +3422,7 @@
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -3397,7 +3439,7 @@
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -3414,7 +3456,7 @@
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -3431,7 +3473,7 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -3448,7 +3490,7 @@
       </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -3465,7 +3507,7 @@
       </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -3482,7 +3524,7 @@
       </c>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -3499,7 +3541,7 @@
       </c>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -3516,7 +3558,7 @@
       </c>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -3533,7 +3575,7 @@
       </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -3550,7 +3592,7 @@
       </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -3567,12 +3609,12 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="130" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>28</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>9</v>
@@ -3584,7 +3626,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -3603,7 +3645,7 @@
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -3624,7 +3666,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="26" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -3643,7 +3685,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" ht="26" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -3662,7 +3704,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -3683,7 +3725,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="26" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -3704,7 +3746,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -3725,12 +3767,12 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="39" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>36</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>9</v>
@@ -3742,7 +3784,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -3759,7 +3801,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1025" ht="52" x14ac:dyDescent="0.35">
       <c r="A40" s="35">
         <v>38</v>
       </c>
@@ -3780,7 +3822,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="52" x14ac:dyDescent="0.35">
       <c r="A41" s="35">
         <v>39</v>
       </c>
@@ -3801,12 +3843,12 @@
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="26" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>40</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C42" s="60" t="s">
         <v>9</v>
@@ -3815,7 +3857,7 @@
         <v>43101</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>12</v>
@@ -4840,18 +4882,18 @@
       <c r="AMJ42" s="17"/>
       <c r="AMK42" s="17"/>
     </row>
-    <row r="43" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A43" s="20">
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="21" t="s">
@@ -5893,28 +5935,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" sqref="A1:G1"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="31" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.54296875" style="31" customWidth="1"/>
+    <col min="7" max="7" width="39.453125" style="31" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -5923,7 +5965,7 @@
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
@@ -5946,11 +5988,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="35">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="65" t="s">
         <v>125</v>
       </c>
       <c r="C3" s="35" t="s">
@@ -5961,11 +6003,11 @@
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="33" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="35">
         <v>2</v>
       </c>
@@ -5976,64 +6018,64 @@
         <v>9</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>115</v>
+        <v>233</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>12</v>
+        <v>236</v>
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="35">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="35" t="s">
+      <c r="E5" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>131</v>
-      </c>
       <c r="F5" s="33" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="35">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="35">
+        <v>5</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>134</v>
-      </c>
       <c r="F6" s="33" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="35">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>9</v>
@@ -6049,12 +6091,12 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="35">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>9</v>
@@ -6070,12 +6112,12 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="35">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>9</v>
@@ -6091,12 +6133,12 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="35">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>138</v>
+      <c r="B10" s="65" t="s">
+        <v>136</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>9</v>
@@ -6108,16 +6150,16 @@
         <v>78</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="35">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>139</v>
+      <c r="B11" s="65" t="s">
+        <v>137</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>9</v>
@@ -6129,16 +6171,16 @@
         <v>78</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="35">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>9</v>
@@ -6149,17 +6191,17 @@
       <c r="E12" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>12</v>
+      <c r="F12" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="35">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>141</v>
+      <c r="B13" s="65" t="s">
+        <v>139</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>9</v>
@@ -6170,17 +6212,17 @@
       <c r="E13" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>12</v>
+      <c r="F13" s="10" t="s">
+        <v>239</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="35">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>142</v>
+      <c r="B14" s="65" t="s">
+        <v>140</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>9</v>
@@ -6188,52 +6230,52 @@
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
       <c r="F14" s="33" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="35">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>143</v>
+      <c r="B15" s="65" t="s">
+        <v>141</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
       <c r="F15" s="33" t="s">
-        <v>12</v>
+        <v>243</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="35">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>145</v>
+      <c r="B16" s="65" t="s">
+        <v>143</v>
       </c>
       <c r="C16" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>146</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="33" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="35">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C17" s="35" t="s">
         <v>9</v>
@@ -6245,54 +6287,54 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="35">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>148</v>
+      <c r="B18" s="65" t="s">
+        <v>146</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
       <c r="F18" s="33" t="s">
-        <v>12</v>
+        <v>240</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="35">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>149</v>
+      <c r="B19" s="65" t="s">
+        <v>147</v>
       </c>
       <c r="C19" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="35" t="s">
         <v>144</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>146</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="33" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="35">
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="33" t="s">
@@ -6300,18 +6342,18 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="35">
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C21" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="33" t="s">
@@ -6319,12 +6361,12 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="35">
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>9</v>
@@ -6338,123 +6380,123 @@
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="35">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>155</v>
+      <c r="B23" s="65" t="s">
+        <v>153</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="35"/>
       <c r="F23" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="35">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>156</v>
+      <c r="B24" s="65" t="s">
+        <v>154</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="35"/>
       <c r="F24" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="35">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>157</v>
+      <c r="B25" s="65" t="s">
+        <v>155</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
       <c r="E25" s="39"/>
       <c r="F25" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="35">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>158</v>
+      <c r="B26" s="65" t="s">
+        <v>156</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="35"/>
       <c r="F26" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A27" s="35">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>159</v>
+      <c r="B27" s="65" t="s">
+        <v>157</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="35"/>
       <c r="F27" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A28" s="35">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>160</v>
+      <c r="B28" s="65" t="s">
+        <v>158</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="35"/>
       <c r="F28" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" s="35">
         <v>27</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>161</v>
+      <c r="B29" s="65" t="s">
+        <v>159</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="35"/>
       <c r="F29" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="35">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>162</v>
+      <c r="B30" s="65" t="s">
+        <v>160</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="35"/>
       <c r="F30" s="33" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G30" s="23"/>
     </row>
@@ -6474,28 +6516,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
       <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="72" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="40" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="40" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="3" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.26953125" style="3" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -6504,7 +6546,7 @@
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
     </row>
-    <row r="2" spans="1:7" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="45" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
@@ -6527,172 +6569,172 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="273" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>166</v>
-      </c>
       <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>169</v>
-      </c>
       <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>172</v>
-      </c>
       <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>7</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>8</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>9</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>9</v>
@@ -6704,12 +6746,12 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>10</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>9</v>
@@ -6721,12 +6763,12 @@
       </c>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>11</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>9</v>
@@ -6738,12 +6780,12 @@
       </c>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>12</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>9</v>
@@ -6755,33 +6797,33 @@
       </c>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>13</v>
       </c>
       <c r="B15" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>188</v>
-      </c>
       <c r="F15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>14</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>9</v>
@@ -6797,12 +6839,12 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>15</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>9</v>
@@ -6818,12 +6860,12 @@
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>16</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>9</v>
@@ -6839,12 +6881,12 @@
       </c>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>17</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>9</v>
@@ -6856,12 +6898,12 @@
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>18</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>9</v>
@@ -6873,75 +6915,75 @@
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>19</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C21" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E21" s="48" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>20</v>
       </c>
       <c r="B22" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>197</v>
-      </c>
       <c r="F22" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>21</v>
       </c>
       <c r="B23" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="C23" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="48" t="s">
-        <v>200</v>
-      </c>
       <c r="F23" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>22</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C24" s="47" t="s">
         <v>9</v>
@@ -6950,19 +6992,19 @@
         <v>64</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>23</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>9</v>
@@ -6972,12 +7014,12 @@
       <c r="F25" s="11"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <v>24</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C26" s="47" t="s">
         <v>9</v>
@@ -6987,21 +7029,21 @@
       <c r="F26" s="11"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <v>25</v>
       </c>
       <c r="B27" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E27" s="49" t="s">
         <v>232</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="49" t="s">
-        <v>233</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>234</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
@@ -7023,20 +7065,20 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="29.5703125" style="3" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="29.54296875" style="3" customWidth="1"/>
+    <col min="8" max="1025" width="9.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -7045,7 +7087,7 @@
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
     </row>
-    <row r="2" spans="1:7" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="45" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
@@ -7068,27 +7110,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="12"/>
@@ -7098,12 +7140,12 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="12"/>
@@ -7113,12 +7155,12 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="12"/>
@@ -7128,12 +7170,12 @@
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="12"/>
@@ -7143,12 +7185,12 @@
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="12"/>
@@ -7158,12 +7200,12 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="12"/>
@@ -7173,12 +7215,12 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" s="52"/>
       <c r="D10" s="12"/>

</xml_diff>

<commit_message>
Changed Configs for ID-Auth
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B6050D6E-A6D2-4B44-B27A-9A695AF93A93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8844" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8850" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="269">
   <si>
     <r>
       <rPr>
@@ -710,12 +711,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t xml:space="preserve">Set up  Authentication Quality Threshold for Fingerprints </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set up  Authentication Quality Threshold for IRIS </t>
-  </si>
-  <si>
     <t xml:space="preserve">Set up  Authentication Quality Threshold for Face/Photo </t>
   </si>
   <si>
@@ -1062,12 +1057,75 @@
   <si>
     <t xml:space="preserve">Documents to be uploaded: Mapping of Applicant Type  Adult/Child + Gender + Foreigner/Local to Document Category + Document Type </t>
   </si>
+  <si>
+    <t>OK
+&lt;15 01 2019&gt;License Key used to set Basic permission of Full/Limited KYC and demo fields through config fields in portal</t>
+  </si>
+  <si>
+    <t>OK
+&lt;15 01 2019&gt;License Key used to set permissable type  of auth for a TSP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;15 01 2019&gt; SI to take care of Data retention</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;15 01 2019&gt; Not in scope for v1</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;15 01 2019&gt; Not in scope for v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up  Authentication Quality Single and Composite Threshold for Fingerprints </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up  Authentication Quality Single and Composite Threshold for IRIS </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1170,6 +1228,20 @@
       <name val="Bookman Old Style"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1366,7 +1438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1583,6 +1655,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1743,60 +1839,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="B2:F9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="B2:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:F9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+  <autoFilter ref="B2:F9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Configuration Feature"/>
-    <tableColumn id="2" name="Type of Config"/>
-    <tableColumn id="3" name="Default Value"/>
-    <tableColumn id="4" name="Other Values"/>
-    <tableColumn id="5" name="Mindtree Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Configuration Feature"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type of Config"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Default Value"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Other Values"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mindtree Comments"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table22" displayName="Table22" ref="A2:G27" totalsRowShown="0">
-  <autoFilter ref="A2:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table22" displayName="Table22" ref="A2:G27" totalsRowShown="0">
+  <autoFilter ref="A2:G27" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="S.No"/>
-    <tableColumn id="2" name="Configuration Feature"/>
-    <tableColumn id="3" name="Type of Config"/>
-    <tableColumn id="4" name="Default Value"/>
-    <tableColumn id="5" name="All Values"/>
-    <tableColumn id="6" name="Mindtree Comments"/>
-    <tableColumn id="7" name="Customer Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="S.No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Configuration Feature"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type of Config"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Default Value"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="All Values"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Mindtree Comments"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Customer Comments"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table224" displayName="Table224" ref="A2:E39" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A2:E39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table224" displayName="Table224" ref="A2:E39" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A2:E39" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="S.No"/>
-    <tableColumn id="2" name="Configuration Feature"/>
-    <tableColumn id="3" name="Type of Config"/>
-    <tableColumn id="4" name="Default Value"/>
-    <tableColumn id="5" name="Other Values"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="S.No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Configuration Feature"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type of Config"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Default Value"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Other Values"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2245" displayName="Table2245" ref="A2:G30" totalsRowShown="0">
-  <autoFilter ref="A2:G30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2245" displayName="Table2245" ref="A2:G30" totalsRowShown="0">
+  <autoFilter ref="A2:G30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="S.No"/>
-    <tableColumn id="2" name="Configuration Feature"/>
-    <tableColumn id="3" name="Type of Config"/>
-    <tableColumn id="4" name="Default Value"/>
-    <tableColumn id="5" name="Other Values"/>
-    <tableColumn id="6" name="Mindtree Comments"/>
-    <tableColumn id="7" name="Customer Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="S.No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Configuration Feature"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Type of Config"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Default Value"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Other Values"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Mindtree Comments"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Customer Comments"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2098,7 +2194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2108,19 +2204,19 @@
       <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="35.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2228,7 @@
       <c r="G1" s="70"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2156,7 +2252,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2192,7 +2288,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2230,7 +2326,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2268,7 +2364,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2306,7 +2402,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2344,7 +2440,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2382,7 +2478,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2420,7 +2516,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -2438,7 +2534,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -2456,7 +2552,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -2476,7 +2572,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -2495,12 +2591,12 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>9</v>
@@ -2514,7 +2610,7 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -2533,7 +2629,7 @@
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -2550,7 +2646,7 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -2582,7 +2678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2590,19 +2686,19 @@
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="16" customWidth="1"/>
     <col min="2" max="2" width="72" style="17" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="16" style="17" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="18" customWidth="1"/>
     <col min="7" max="7" width="39" style="18" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>29</v>
       </c>
@@ -2613,7 +2709,7 @@
       <c r="F1" s="71"/>
       <c r="G1" s="71"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -2636,7 +2732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -2657,12 +2753,12 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" s="22" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -2676,7 +2772,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -2697,7 +2793,7 @@
       </c>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -2718,7 +2814,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -2739,7 +2835,7 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -2760,7 +2856,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" s="22" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="22" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -2771,7 +2867,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="21" t="s">
@@ -2779,7 +2875,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -2796,7 +2892,7 @@
       </c>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -2813,7 +2909,7 @@
       </c>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -2830,7 +2926,7 @@
       </c>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -2847,7 +2943,7 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -2864,7 +2960,7 @@
       </c>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -2881,7 +2977,7 @@
       </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -2898,7 +2994,7 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -2915,7 +3011,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -2932,7 +3028,7 @@
       </c>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -2953,7 +3049,7 @@
       </c>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -2970,7 +3066,7 @@
       </c>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -2987,7 +3083,7 @@
       </c>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="1:7" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -3006,7 +3102,7 @@
       </c>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -3025,7 +3121,7 @@
       </c>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -3042,7 +3138,7 @@
       </c>
       <c r="G24" s="21"/>
     </row>
-    <row r="25" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -3061,7 +3157,7 @@
       </c>
       <c r="G25" s="21"/>
     </row>
-    <row r="26" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="57">
         <v>24</v>
       </c>
@@ -3072,7 +3168,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="58" t="s">
@@ -3080,12 +3176,12 @@
       </c>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C27" s="60" t="s">
         <v>9</v>
@@ -3094,25 +3190,25 @@
         <v>43101</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F27" s="58" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="56"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="21" t="s">
@@ -3120,7 +3216,7 @@
       </c>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>66</v>
       </c>
@@ -3139,27 +3235,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="31" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="60.5546875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="44.5546875" style="17" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
         <v>67</v>
       </c>
@@ -3170,7 +3266,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
@@ -3193,7 +3289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3210,11 +3306,11 @@
         <v>70</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -3235,7 +3331,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -3248,11 +3344,11 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -3269,7 +3365,7 @@
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -3286,11 +3382,11 @@
         <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -3311,7 +3407,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3332,7 +3428,7 @@
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3353,7 +3449,7 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3374,7 +3470,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3395,7 +3491,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3416,7 +3512,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3430,19 +3526,19 @@
         <v>69</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>9</v>
@@ -3451,14 +3547,14 @@
         <v>69</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -3475,7 +3571,7 @@
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -3492,7 +3588,7 @@
       </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -3509,7 +3605,7 @@
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -3526,7 +3622,7 @@
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="63">
         <v>18</v>
       </c>
@@ -3543,7 +3639,7 @@
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="63">
         <v>19</v>
       </c>
@@ -3560,7 +3656,7 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -3577,7 +3673,7 @@
       </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -3594,7 +3690,7 @@
       </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="63">
         <v>22</v>
       </c>
@@ -3611,7 +3707,7 @@
       </c>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="63">
         <v>23</v>
       </c>
@@ -3628,7 +3724,7 @@
       </c>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -3645,7 +3741,7 @@
       </c>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -3662,7 +3758,7 @@
       </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -3679,12 +3775,12 @@
       </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C29" s="33" t="s">
         <v>9</v>
@@ -3696,12 +3792,12 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="132" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>9</v>
@@ -3713,7 +3809,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -3732,7 +3828,7 @@
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -3753,7 +3849,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -3772,7 +3868,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -3791,7 +3887,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -3802,17 +3898,17 @@
         <v>9</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -3833,7 +3929,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -3854,12 +3950,12 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>9</v>
@@ -3871,7 +3967,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -3888,12 +3984,12 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="35">
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>9</v>
@@ -3902,19 +3998,19 @@
         <v>69</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>39</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>9</v>
@@ -3923,19 +4019,19 @@
         <v>69</v>
       </c>
       <c r="E41" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>40</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C42" s="46" t="s">
         <v>9</v>
@@ -3944,7 +4040,7 @@
         <v>43466</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>12</v>
@@ -4969,18 +5065,18 @@
       <c r="AMJ42" s="17"/>
       <c r="AMK42" s="17"/>
     </row>
-    <row r="43" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
@@ -6006,29 +6102,29 @@
       <c r="AMJ43" s="17"/>
       <c r="AMK43" s="17"/>
     </row>
-    <row r="44" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>42</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C44" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="67"/>
       <c r="G44" s="66"/>
     </row>
-    <row r="45" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>43</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C45" s="47" t="s">
         <v>9</v>
@@ -6040,114 +6136,114 @@
       <c r="F45" s="67"/>
       <c r="G45" s="66"/>
     </row>
-    <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>44</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C46" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="67"/>
       <c r="G46" s="66"/>
     </row>
-    <row r="47" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>45</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C47" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="67"/>
       <c r="G47" s="66"/>
     </row>
-    <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A48" s="35">
         <v>46</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C48" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="46" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="67"/>
       <c r="G48" s="66"/>
     </row>
-    <row r="49" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>47</v>
       </c>
       <c r="B49" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="46" t="s">
         <v>249</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="46" t="s">
-        <v>251</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="67"/>
       <c r="G49" s="66"/>
     </row>
-    <row r="50" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="35">
         <v>48</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C50" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="46" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="67"/>
       <c r="G50" s="66"/>
     </row>
-    <row r="51" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>49</v>
       </c>
       <c r="B51" s="46" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C51" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="46" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E51" s="46"/>
       <c r="F51" s="67"/>
       <c r="G51" s="66"/>
     </row>
-    <row r="52" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="35">
         <v>50</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C52" s="47" t="s">
         <v>9</v>
@@ -6159,12 +6255,12 @@
       <c r="F52" s="67"/>
       <c r="G52" s="66"/>
     </row>
-    <row r="53" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="35">
         <v>51</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C53" s="47" t="s">
         <v>9</v>
@@ -6176,12 +6272,12 @@
       <c r="F53" s="67"/>
       <c r="G53" s="66"/>
     </row>
-    <row r="54" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="35">
         <v>52</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C54" s="47" t="s">
         <v>9</v>
@@ -6193,12 +6289,12 @@
       <c r="F54" s="67"/>
       <c r="G54" s="66"/>
     </row>
-    <row r="55" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="35">
         <v>53</v>
       </c>
       <c r="B55" s="46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C55" s="47" t="s">
         <v>9</v>
@@ -6210,12 +6306,12 @@
       <c r="F55" s="67"/>
       <c r="G55" s="66"/>
     </row>
-    <row r="56" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="35">
         <v>54</v>
       </c>
       <c r="B56" s="69" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C56" s="47" t="s">
         <v>9</v>
@@ -6225,18 +6321,18 @@
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
     </row>
-    <row r="57" spans="1:7" ht="132" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>55</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C57" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E57" s="51"/>
       <c r="F57" s="66"/>
@@ -6255,7 +6351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6265,21 +6361,21 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5546875" style="31" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" style="31" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="31" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" style="31" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="72"/>
@@ -6288,7 +6384,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
@@ -6311,7 +6407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="35">
         <v>1</v>
       </c>
@@ -6326,11 +6422,11 @@
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>2</v>
       </c>
@@ -6341,17 +6437,17 @@
         <v>9</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E4" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>226</v>
-      </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>3</v>
       </c>
@@ -6372,7 +6468,7 @@
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
         <v>4</v>
       </c>
@@ -6393,7 +6489,7 @@
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>5</v>
       </c>
@@ -6414,7 +6510,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>6</v>
       </c>
@@ -6435,7 +6531,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>7</v>
       </c>
@@ -6456,7 +6552,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>8</v>
       </c>
@@ -6473,11 +6569,11 @@
         <v>78</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>9</v>
       </c>
@@ -6494,11 +6590,11 @@
         <v>78</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>10</v>
       </c>
@@ -6515,11 +6611,11 @@
         <v>78</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>11</v>
       </c>
@@ -6536,11 +6632,11 @@
         <v>78</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>12</v>
       </c>
@@ -6553,11 +6649,11 @@
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
       <c r="F14" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>13</v>
       </c>
@@ -6570,11 +6666,11 @@
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
       <c r="F15" s="33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>14</v>
       </c>
@@ -6589,11 +6685,11 @@
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>15</v>
       </c>
@@ -6610,7 +6706,7 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>16</v>
       </c>
@@ -6623,11 +6719,11 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
       <c r="F18" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>17</v>
       </c>
@@ -6642,11 +6738,11 @@
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>18</v>
       </c>
@@ -6665,7 +6761,7 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>19</v>
       </c>
@@ -6684,7 +6780,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>20</v>
       </c>
@@ -6703,7 +6799,7 @@
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>21</v>
       </c>
@@ -6714,11 +6810,11 @@
       <c r="D23" s="7"/>
       <c r="E23" s="35"/>
       <c r="F23" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>22</v>
       </c>
@@ -6729,11 +6825,11 @@
       <c r="D24" s="7"/>
       <c r="E24" s="35"/>
       <c r="F24" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>23</v>
       </c>
@@ -6744,11 +6840,11 @@
       <c r="D25" s="23"/>
       <c r="E25" s="39"/>
       <c r="F25" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>24</v>
       </c>
@@ -6759,11 +6855,11 @@
       <c r="D26" s="7"/>
       <c r="E26" s="35"/>
       <c r="F26" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>25</v>
       </c>
@@ -6774,11 +6870,11 @@
       <c r="D27" s="7"/>
       <c r="E27" s="35"/>
       <c r="F27" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>26</v>
       </c>
@@ -6789,11 +6885,11 @@
       <c r="D28" s="7"/>
       <c r="E28" s="35"/>
       <c r="F28" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>27</v>
       </c>
@@ -6804,11 +6900,11 @@
       <c r="D29" s="7"/>
       <c r="E29" s="35"/>
       <c r="F29" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>28</v>
       </c>
@@ -6819,7 +6915,7 @@
       <c r="D30" s="7"/>
       <c r="E30" s="35"/>
       <c r="F30" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G30" s="23"/>
     </row>
@@ -6836,29 +6932,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="72" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="40" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" style="3" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="40" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="3" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
         <v>153</v>
       </c>
@@ -6869,7 +6965,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
     </row>
-    <row r="2" spans="1:7" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
@@ -6892,7 +6988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="277.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -6909,11 +7005,11 @@
         <v>156</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>12</v>
+        <v>262</v>
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -6930,129 +7026,129 @@
         <v>159</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>12</v>
+        <v>263</v>
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="48" t="s">
+      <c r="C5" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>12</v>
+      <c r="F5" s="77" t="s">
+        <v>264</v>
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="74"/>
+      <c r="D6" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="50" t="s">
+      <c r="C7" s="74"/>
+      <c r="D7" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="73" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="48" t="s">
+      <c r="C8" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="73" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="50" t="s">
+      <c r="C9" s="74"/>
+      <c r="D9" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="73" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="50" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="76" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="73" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>9</v>
       </c>
@@ -7069,7 +7165,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>10</v>
       </c>
@@ -7086,7 +7182,7 @@
       </c>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>11</v>
       </c>
@@ -7103,7 +7199,7 @@
       </c>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>12</v>
       </c>
@@ -7120,7 +7216,7 @@
       </c>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>13</v>
       </c>
@@ -7141,12 +7237,12 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>14</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>9</v>
@@ -7162,12 +7258,12 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>15</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>180</v>
+        <v>268</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>9</v>
@@ -7183,12 +7279,12 @@
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>16</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>9</v>
@@ -7204,12 +7300,12 @@
       </c>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>17</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>9</v>
@@ -7221,12 +7317,12 @@
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>18</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C20" s="47" t="s">
         <v>9</v>
@@ -7238,75 +7334,75 @@
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="78">
         <v>19</v>
       </c>
-      <c r="B21" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="48" t="s">
+      <c r="B21" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>12</v>
+      <c r="F21" s="77" t="s">
+        <v>265</v>
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>20</v>
       </c>
       <c r="B22" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>187</v>
-      </c>
       <c r="F22" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>21</v>
       </c>
       <c r="B23" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="C23" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="E23" s="48" t="s">
-        <v>190</v>
-      </c>
       <c r="F23" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>22</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C24" s="47" t="s">
         <v>9</v>
@@ -7315,19 +7411,19 @@
         <v>64</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>23</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>9</v>
@@ -7337,12 +7433,12 @@
       <c r="F25" s="11"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>24</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C26" s="47" t="s">
         <v>9</v>
@@ -7352,23 +7448,25 @@
       <c r="F26" s="11"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="80" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" s="80" t="s">
         <v>220</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="F27" s="11"/>
+      <c r="F27" s="11" t="s">
+        <v>266</v>
+      </c>
       <c r="G27" s="12"/>
     </row>
   </sheetData>
@@ -7381,27 +7479,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="29.5546875" style="3" customWidth="1"/>
-    <col min="8" max="1025" width="9.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="29.5703125" style="3" customWidth="1"/>
+    <col min="8" max="1025" width="9.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="72"/>
@@ -7410,7 +7508,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
     </row>
-    <row r="2" spans="1:7" s="45" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
@@ -7433,27 +7531,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="12"/>
@@ -7463,12 +7561,12 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="12"/>
@@ -7478,12 +7576,12 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="12"/>
@@ -7493,12 +7591,12 @@
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="12"/>
@@ -7508,12 +7606,12 @@
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="12"/>
@@ -7523,12 +7621,12 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="12"/>
@@ -7538,12 +7636,12 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C10" s="52"/>
       <c r="D10" s="12"/>

</xml_diff>